<commit_message>
updates May 23 with pics
</commit_message>
<xml_diff>
--- a/ZFS/zfs-parts-list-60TB-backup-raidz1.xlsx
+++ b/ZFS/zfs-parts-list-60TB-backup-raidz1.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1-zfs-parts-list" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Info" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -26,13 +26,14 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Parts list without drives</t>
         </r>
@@ -43,9 +44,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
-  <si>
-    <t xml:space="preserve">60TB ZFS backup 2023.0502</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">60TB ZFS backup 2023.0523</t>
   </si>
   <si>
     <t xml:space="preserve">Price/ea</t>
@@ -78,7 +79,25 @@
     <t xml:space="preserve">https://www.ebay.com/itm/404020493983</t>
   </si>
   <si>
-    <t xml:space="preserve">HBA SAS x8E IT mode pcie</t>
+    <t xml:space="preserve">https://www.amazon.com/dp/B0BQN2NLBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC power supply, 6x SATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/Enermax-Cyberbron-ECB500AWT-Non-Modular-Warranty/dp/B08K1ZBYPZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALT: PC Power supply, 8x SATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B004OVG24Y/?coliid=I1E7VJ7AVOQT0A&amp;colid=1W550CE142KLT&amp;psc=1&amp;ref_=lv_ov_lig_dp_it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifications Mfr Part Number: EP-700PM Features: 75% Efficiency Rating Maximum Power: 700W Input: Input Voltage: 115 230 V Connectors: 1x 20+4pin Main Power Connector, 1x 4+4pin ATX Power Connector, 1x 6pin PCI-Express Connector, 1x 6+2pin PCI-Express Connector, 8x SATA Connectors, 8x 4pin Molex Connectors, 2x FDD Connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBA SAS x8E IT mode pcie card</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.ebay.com/sch/i.html?_from=R40&amp;_nkw=sas9200-8e+IT+mode&amp;_sacat=0&amp;LH_TitleDesc=0&amp;LH_PrefLoc=2&amp;_sop=15</t>
@@ -108,16 +127,16 @@
     <t xml:space="preserve">https://www.amazon.com/Toshiba-258014-Mg09aca18te-7200rpm-512mib/dp/B093Z5LFWD</t>
   </si>
   <si>
-    <t xml:space="preserve">PC power supply, 6x SATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/Enermax-Cyberbron-ECB500AWT-Non-Modular-Warranty/dp/B08K1ZBYPZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC Power supply, 8x SATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/dp/B004OVG24Y/?coliid=I1E7VJ7AVOQT0A&amp;colid=1W550CE142KLT&amp;psc=1&amp;ref_=lv_ov_lig_dp_it</t>
+    <t xml:space="preserve">ALT: 12TB NAS drives (x8) -2 for RAIDZ2 parity = ~72TB, use wintelguy calc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/Seagate-IronWolf-12TB-Internal-Drive/dp/B084ZV1DN6?th=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung T7 500GB USB3 boot/root drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/dp/B0874XJL6M/ref=twister_B0B79D1NQ6?_encoding=UTF8&amp;th=1</t>
   </si>
   <si>
     <t xml:space="preserve">UPS, 700VA/370W x8 outlets</t>
@@ -126,7 +145,7 @@
     <t xml:space="preserve">https://www.amazon.com/gp/product/B07SKX78PV/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
-    <t xml:space="preserve">Refurb PC w/ 4x pcie slot – Dell Optiplex 7040 SFF – 16GB RAM, Quad-core-i5 with HDMI</t>
+    <t xml:space="preserve">Turnkey Refurb PC w/ 4x pcie slot – Dell Optiplex 7040 SFF – 16GB RAM, Quad-core-i5 with HDMI</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.ebay.com/itm/304041042675?_trkparms=ispr%3D5&amp;hash=item46ca4222f3:g:YVYAAOSwCJVh~cDu</t>
@@ -144,7 +163,7 @@
     <t xml:space="preserve">RAIDZ1 18000 , 5 drives, slop space, 5% free space, ~60TiB actual usable space before compression</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE RAIDZ2 (at least) with 6+ drives is strongly recommended for long-term usage</t>
+    <t xml:space="preserve">NOTE RAIDZ2 (at least) with 6+ drives is strongly recommended for long-term usage; if you buy the 5-bay enclosure it is a good complement to the HDDRACK and supports up to 8-10 drives on (1) power supply</t>
   </si>
   <si>
     <t xml:space="preserve">Grand Total</t>
@@ -156,6 +175,9 @@
     <t xml:space="preserve">2023 Parts list for entry-level ZFS backup / fileserver</t>
   </si>
   <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
     <t xml:space="preserve">By Kingneutron</t>
   </si>
   <si>
@@ -171,6 +193,9 @@
     <t xml:space="preserve">For longer-term backup solution, go with at least RAIDZ2 at the 6+ drive mark to avoid too many disks failing during rebuild / data loss</t>
   </si>
   <si>
+    <t xml:space="preserve">The 5x18TB drive RAIDZ1 is an attempt to get the whole system under $2k for a homelab</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cooling the HBA PCIe card:</t>
   </si>
   <si>
@@ -181,6 +206,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dell Optiplex 7040 SFF Owners Manual with motherboard info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.reddit.com/r/zfs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZFS forum, ask questions here</t>
   </si>
 </sst>
 </file>
@@ -191,11 +222,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -217,46 +249,82 @@
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="15"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -264,6 +332,7 @@
       <color rgb="FFEEEEEE"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -325,114 +394,148 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -515,15 +618,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>27360</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>5764320</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7097400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -536,8 +639,452 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4764600" y="3180960"/>
-          <a:ext cx="8059680" cy="6030720"/>
+          <a:off x="4737240" y="14873760"/>
+          <a:ext cx="7097400" cy="5794560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>852120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="1122120"/>
+          <a:ext cx="988560" cy="852120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>816840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="205200"/>
+          <a:ext cx="816840" cy="917280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>837720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="2039040"/>
+          <a:ext cx="988560" cy="837720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>735120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="5072400"/>
+          <a:ext cx="988560" cy="735120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>673200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="5989320"/>
+          <a:ext cx="988560" cy="673200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>609840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="6906240"/>
+          <a:ext cx="988560" cy="609840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>936720</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="7820640"/>
+          <a:ext cx="936720" cy="914760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>651240</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 9" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="8735040"/>
+          <a:ext cx="651240" cy="914760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>649800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 10" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="9649440"/>
+          <a:ext cx="649800" cy="914760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>605520</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 11" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId11"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="10563840"/>
+          <a:ext cx="605520" cy="914760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>655560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 12" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="11478240"/>
+          <a:ext cx="988560" cy="655560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>941760</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 13" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14700240" y="12392640"/>
+          <a:ext cx="941760" cy="914760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -557,10 +1104,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="456.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,9 +1118,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="5.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="114.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="66.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="105.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="36.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,7 +1146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="72.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -615,11 +1164,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="72.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="8" t="n">
         <v>98</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -632,226 +1181,282 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="72.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="8" t="n">
-        <v>50</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>40</v>
+      </c>
+      <c r="C4" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="6" t="n">
         <f aca="false">B4*C4</f>
-        <v>50</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="166.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>0</v>
       </c>
       <c r="D5" s="6" t="n">
         <f aca="false">B5*C5</f>
-        <v>34</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="F5" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="72.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" s="15" t="n">
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="6" t="n">
         <f aca="false">B6*C6</f>
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="72.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6" t="n">
         <f aca="false">B7*C7</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="12" t="n">
-        <v>288</v>
-      </c>
-      <c r="C8" s="13" t="n">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D8" s="6" t="n">
         <f aca="false">B8*C8</f>
-        <v>1440</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="12" t="n">
-        <v>40</v>
-      </c>
-      <c r="C9" s="13" t="n">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="D9" s="6" t="n">
         <f aca="false">B9*C9</f>
-        <v>40</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="14" t="n">
-        <v>70</v>
-      </c>
-      <c r="C10" s="15" t="n">
         <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>288</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>5</v>
       </c>
       <c r="D10" s="6" t="n">
         <f aca="false">B10*C10</f>
+        <v>1440</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="19" t="n">
+        <v>225</v>
+      </c>
+      <c r="C11" s="13" t="n">
         <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>80</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>1</v>
       </c>
       <c r="D11" s="6" t="n">
         <f aca="false">B11*C11</f>
-        <v>80</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>170</v>
-      </c>
-      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="22" t="n">
+        <v>70</v>
+      </c>
+      <c r="C12" s="23" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="6" t="n">
         <f aca="false">B12*C12</f>
+        <v>70</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>80</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <f aca="false">B13*C13</f>
+        <v>80</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="6" t="n">
         <v>170</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="C14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <f aca="false">B14*C14</f>
+        <v>170</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="6" t="n">
-        <f aca="false">SUM(D2:D16)</f>
-        <v>1871</v>
-      </c>
-      <c r="E17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="19" t="n">
-        <f aca="false">SUM(D2:D12)-D8</f>
-        <v>431</v>
-      </c>
-      <c r="E18" s="20"/>
-    </row>
+      <c r="B15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="49.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <f aca="false">SUM(D2:D18)</f>
+        <v>1941</v>
+      </c>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="27" t="n">
+        <f aca="false">SUM(D2:D14)-SUM(D10:D11)</f>
+        <v>501</v>
+      </c>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId2" display="https://www.amazon.com/CableCreation-External-26pin-SFF-8088-Cable/dp/B07CL2V1B8"/>
-    <hyperlink ref="E8" r:id="rId3" display="https://www.amazon.com/Toshiba-258014-Mg09aca18te-7200rpm-512mib/dp/B093Z5LFWD"/>
-    <hyperlink ref="E9" r:id="rId4" display="https://www.amazon.com/Enermax-Cyberbron-ECB500AWT-Non-Modular-Warranty/dp/B08K1ZBYPZ"/>
-    <hyperlink ref="E12" r:id="rId5" display="https://www.ebay.com/itm/304041042675?_trkparms=ispr%3D5&amp;hash=item46ca4222f3:g:YVYAAOSwCJVh~cDu"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.amazon.com/dp/B0BQN2NLBL"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://www.amazon.com/Enermax-Cyberbron-ECB500AWT-Non-Modular-Warranty/dp/B08K1ZBYPZ"/>
+    <hyperlink ref="E7" r:id="rId4" display="https://www.amazon.com/CableCreation-External-26pin-SFF-8088-Cable/dp/B07CL2V1B8"/>
+    <hyperlink ref="E10" r:id="rId5" display="https://www.amazon.com/Toshiba-258014-Mg09aca18te-7200rpm-512mib/dp/B093Z5LFWD"/>
+    <hyperlink ref="E14" r:id="rId6" display="https://www.ebay.com/itm/304041042675?_trkparms=ispr%3D5&amp;hash=item46ca4222f3:g:YVYAAOSwCJVh~cDu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -860,8 +1465,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <drawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -870,65 +1475,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="64.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="82.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>36</v>
+      <c r="A1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>37</v>
+      <c r="A2" s="30" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>39</v>
+      <c r="A3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
-        <v>40</v>
+      <c r="A5" s="32" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
-        <v>41</v>
+      <c r="A6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>43</v>
+      <c r="A8" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>44</v>
+      <c r="B9" s="21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
-        <v>45</v>
+      <c r="A11" s="31" t="s">
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>